<commit_message>
Update reg DF case study
</commit_message>
<xml_diff>
--- a/regionalization_df/rice_inventory.xlsx
+++ b/regionalization_df/rice_inventory.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10910"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmutel/Code/regionalized-lca-examples/discussion_forum/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmutel/Code/regionalized-lca-examples/regionalization_df/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7D6EF4D-BAAF-3243-A267-B74427BC7C9E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E5F821-33EB-0547-B245-AC532ACF2360}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="60">
   <si>
     <t>Database</t>
   </si>
@@ -82,9 +82,6 @@
     <t>AWARE Case Study</t>
   </si>
   <si>
-    <t>rice, at farm</t>
-  </si>
-  <si>
     <t>CN</t>
   </si>
   <si>
@@ -97,39 +94,21 @@
     <t>m3</t>
   </si>
   <si>
-    <t>ecoinvent</t>
-  </si>
-  <si>
     <t>CH</t>
   </si>
   <si>
-    <t>maize starch effluent, to WWTP , class 2</t>
-  </si>
-  <si>
-    <t>Natural gas, burned in industrial furnace &gt;100kW</t>
-  </si>
-  <si>
     <t>MJ</t>
   </si>
   <si>
     <t>RER</t>
   </si>
   <si>
-    <t>Transport, lorry &gt;32t, EURO3</t>
-  </si>
-  <si>
     <t>tkm</t>
   </si>
   <si>
-    <t>Tap water, at user</t>
-  </si>
-  <si>
     <t>GLO</t>
   </si>
   <si>
-    <t>Electricity, medium voltage, at grid</t>
-  </si>
-  <si>
     <t>kWh</t>
   </si>
   <si>
@@ -142,12 +121,6 @@
     <t>Packed rice CN</t>
   </si>
   <si>
-    <t>Packaging film, LDPE, at plant</t>
-  </si>
-  <si>
-    <t>Packaging, corr board, mixed fibre, at plant</t>
-  </si>
-  <si>
     <t>white rice, at supermarket</t>
   </si>
   <si>
@@ -160,9 +133,6 @@
     <t>Cooked rice CN</t>
   </si>
   <si>
-    <t>Electricity, low voltage, at grid</t>
-  </si>
-  <si>
     <t>Transport, regular bus</t>
   </si>
   <si>
@@ -181,28 +151,77 @@
     <t>Supermarket rice CH</t>
   </si>
   <si>
-    <t>Transport, transoceanic freight ship</t>
-  </si>
-  <si>
-    <t>Transport, lorry &gt;32t, EURO5</t>
-  </si>
-  <si>
     <t>Cooked rice CH</t>
   </si>
   <si>
-    <t>natural gas, burned in gas stove</t>
-  </si>
-  <si>
-    <t>Transport, passenger car, diesel, EURO5</t>
+    <t>ecoinvent 3.5 cutoff</t>
+  </si>
+  <si>
+    <t>RoW</t>
+  </si>
+  <si>
+    <t>﻿rice production</t>
+  </si>
+  <si>
+    <t>reference product</t>
+  </si>
+  <si>
+    <t>rice</t>
+  </si>
+  <si>
+    <t>heat production, natural gas, at industrial furnace &gt;100kW</t>
+  </si>
+  <si>
+    <t>market for tap water</t>
+  </si>
+  <si>
+    <t>transport, freight, lorry &gt;32 metric ton, EURO3</t>
+  </si>
+  <si>
+    <t>market group for electricity, medium voltage</t>
+  </si>
+  <si>
+    <t>market group for electricity, low voltage</t>
+  </si>
+  <si>
+    <t>rice production</t>
+  </si>
+  <si>
+    <t>market for packaging film, low density polyethylene</t>
+  </si>
+  <si>
+    <t>market for corrugated board box</t>
+  </si>
+  <si>
+    <t>treatment of wastewater from maize starch production, capacity 1.1E10l/year</t>
+  </si>
+  <si>
+    <t>transport, freight, sea, transoceanic ship</t>
+  </si>
+  <si>
+    <t>market for heat, central or small-scale, natural gas</t>
+  </si>
+  <si>
+    <t>transport, passenger car, large size, diesel, EURO 5</t>
+  </si>
+  <si>
+    <t>km</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -247,6 +266,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -267,28 +293,33 @@
   </borders>
   <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -603,67 +634,73 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F63"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="50.6640625" customWidth="1"/>
-    <col min="2" max="2" width="70.33203125" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" customWidth="1"/>
-    <col min="4" max="4" width="30.6640625" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" customWidth="1"/>
+    <col min="2" max="3" width="70.33203125" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+    <col min="5" max="5" width="30.6640625" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="2"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C1" s="1"/>
+      <c r="D1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="D2" s="2"/>
+    </row>
+    <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="2"/>
+      <c r="E4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -671,7 +708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -679,7 +716,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -687,12 +724,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -700,185 +737,193 @@
         <v>12</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="E13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E13" t="s">
-        <v>19</v>
-      </c>
       <c r="F13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>25</v>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>55</v>
       </c>
       <c r="B14">
         <v>9.7446000000000002E-4</v>
       </c>
-      <c r="C14" t="s">
-        <v>22</v>
-      </c>
       <c r="D14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E14" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F14" t="s">
+        <v>43</v>
+      </c>
+      <c r="G14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="B15">
         <v>1.3441000000000001</v>
       </c>
       <c r="C15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" t="s">
         <v>9</v>
       </c>
-      <c r="D15" t="s">
-        <v>23</v>
-      </c>
       <c r="E15" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="F15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="G15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="B16">
         <v>1.0550999999999999</v>
       </c>
-      <c r="C16" t="s">
-        <v>27</v>
-      </c>
       <c r="D16" t="s">
         <v>23</v>
       </c>
       <c r="E16" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="F16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>29</v>
+        <v>43</v>
+      </c>
+      <c r="G16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="B17">
         <v>6.7204E-2</v>
       </c>
-      <c r="C17" t="s">
-        <v>30</v>
-      </c>
       <c r="D17" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E17" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="F17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="G17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="B18">
         <v>9.7446000000000002E-4</v>
       </c>
-      <c r="C18" t="s">
-        <v>35</v>
-      </c>
       <c r="D18" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="E18" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="F18" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+      <c r="G18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="B19">
         <v>0.17136999999999999</v>
       </c>
-      <c r="C19" t="s">
-        <v>34</v>
-      </c>
       <c r="D19" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E19" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="F19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="G19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" s="2"/>
-    </row>
-    <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>3</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C22" s="2"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -886,7 +931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -894,7 +939,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -902,12 +947,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>11</v>
       </c>
@@ -915,131 +960,138 @@
         <v>12</v>
       </c>
       <c r="C29" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="F29" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="G29" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B30" s="3">
         <v>1</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>35</v>
-      </c>
+      <c r="C30" s="3"/>
       <c r="D30" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E30" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="F30" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G30" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="F30" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>9</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="E31" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E31" t="s">
-        <v>19</v>
-      </c>
       <c r="F31" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="G31" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B32">
         <v>0.01</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>9</v>
       </c>
-      <c r="D32" t="s">
-        <v>23</v>
-      </c>
       <c r="E32" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="F32" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="G32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="B33">
         <v>0.05</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>9</v>
       </c>
-      <c r="D33" t="s">
-        <v>23</v>
-      </c>
       <c r="E33" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="F33" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+      <c r="G33" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
-    </row>
-    <row r="35" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="E34" s="5"/>
+    </row>
+    <row r="35" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C35" s="2"/>
-    </row>
-    <row r="36" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+      <c r="C35" s="3"/>
+      <c r="D35" s="2"/>
+    </row>
+    <row r="36" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>3</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C36" s="2"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+      <c r="C36" s="3"/>
+      <c r="D36" s="2"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>4</v>
       </c>
       <c r="B37" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>5</v>
       </c>
@@ -1047,7 +1099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>6</v>
       </c>
@@ -1055,7 +1107,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>8</v>
       </c>
@@ -1063,12 +1115,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>11</v>
       </c>
@@ -1076,109 +1128,116 @@
         <v>12</v>
       </c>
       <c r="C43" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="E43" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="F43" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F43" s="1" t="s">
+      <c r="G43" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B44" s="3">
         <v>1</v>
       </c>
-      <c r="C44" s="3" t="s">
-        <v>35</v>
-      </c>
+      <c r="C44" s="3"/>
       <c r="D44" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E44" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E44" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F44" t="s">
+      <c r="F44" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G44" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B45">
         <v>1</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
         <v>9</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="E45" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E45" t="s">
-        <v>19</v>
-      </c>
       <c r="F45" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A46" s="4" t="s">
-        <v>29</v>
+        <v>18</v>
+      </c>
+      <c r="G45" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="B46">
         <v>1.3</v>
       </c>
-      <c r="C46" t="s">
-        <v>30</v>
-      </c>
       <c r="D46" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E46" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="F46" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="G46" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="5"/>
       <c r="B47" s="5"/>
-    </row>
-    <row r="48" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="C47" s="5"/>
+    </row>
+    <row r="48" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C48" s="2"/>
-    </row>
-    <row r="49" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+      <c r="C48" s="3"/>
+      <c r="D48" s="2"/>
+    </row>
+    <row r="49" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>3</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C49" s="2"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="C49" s="3"/>
+      <c r="D49" s="2"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>4</v>
       </c>
       <c r="B50" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>5</v>
       </c>
@@ -1186,7 +1245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>6</v>
       </c>
@@ -1194,7 +1253,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>8</v>
       </c>
@@ -1202,12 +1261,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>11</v>
       </c>
@@ -1215,127 +1274,136 @@
         <v>12</v>
       </c>
       <c r="C56" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D56" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="E56" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E56" s="1" t="s">
+      <c r="F56" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F56" s="1" t="s">
+      <c r="G56" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B57" s="3">
         <v>1</v>
       </c>
-      <c r="C57" s="3" t="s">
-        <v>35</v>
-      </c>
+      <c r="C57" s="3"/>
       <c r="D57" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E57" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E57" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F57" t="s">
+      <c r="F57" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G57" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B58">
         <v>0.7</v>
       </c>
-      <c r="C58" t="s">
+      <c r="D58" t="s">
         <v>9</v>
       </c>
-      <c r="D58" s="3" t="s">
+      <c r="E58" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E58" t="s">
-        <v>19</v>
-      </c>
       <c r="F58" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59" s="5" t="s">
-        <v>44</v>
+        <v>18</v>
+      </c>
+      <c r="G58" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>51</v>
       </c>
       <c r="B59" s="5">
         <v>0.3</v>
       </c>
-      <c r="C59" t="s">
-        <v>34</v>
-      </c>
+      <c r="C59" s="5"/>
       <c r="D59" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E59" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="F59" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" s="5" t="s">
-        <v>31</v>
+        <v>18</v>
+      </c>
+      <c r="G59" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A60" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="B60" s="5">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="5"/>
+      <c r="D60" t="s">
+        <v>28</v>
+      </c>
+      <c r="E60" t="s">
+        <v>42</v>
+      </c>
+      <c r="F60" t="s">
+        <v>43</v>
+      </c>
+      <c r="G60" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A61" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="D60" t="s">
-        <v>23</v>
-      </c>
-      <c r="E60" t="s">
-        <v>32</v>
-      </c>
-      <c r="F60" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A61" s="4" t="s">
-        <v>45</v>
       </c>
       <c r="B61" s="4">
         <v>0.42</v>
       </c>
-      <c r="C61" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D61" t="s">
-        <v>23</v>
+      <c r="C61" s="4"/>
+      <c r="D61" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="E61" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F61" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+      <c r="G61" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="4"/>
       <c r="B62" s="4"/>
-      <c r="C62" s="5"/>
-    </row>
-    <row r="63" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="C62" s="4"/>
+      <c r="D62" s="5"/>
+    </row>
+    <row r="63" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="4"/>
       <c r="B63" s="5"/>
-      <c r="C63" s="4"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1350,49 +1418,51 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1528DE61-51B6-774C-B1EA-9005B1C9216F}">
-  <dimension ref="A1:F61"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="50.6640625" customWidth="1"/>
-    <col min="2" max="2" width="70.33203125" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" customWidth="1"/>
-    <col min="4" max="4" width="30.6640625" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" customWidth="1"/>
+    <col min="2" max="3" width="70.33203125" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+    <col min="5" max="5" width="30.6640625" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="2"/>
-    </row>
-    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1400,7 +1470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1408,7 +1478,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1416,12 +1486,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -1429,185 +1499,193 @@
         <v>12</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="E10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E10" t="s">
-        <v>47</v>
-      </c>
       <c r="F10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>25</v>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>55</v>
       </c>
       <c r="B11">
         <v>9.7446000000000002E-4</v>
       </c>
-      <c r="C11" t="s">
-        <v>22</v>
-      </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E11" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F11" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="B12">
         <v>1.3441000000000001</v>
       </c>
       <c r="C12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" t="s">
         <v>9</v>
       </c>
-      <c r="D12" t="s">
-        <v>23</v>
-      </c>
       <c r="E12" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>47</v>
-      </c>
-      <c r="F12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>26</v>
       </c>
       <c r="B13">
         <v>1.0550999999999999</v>
       </c>
-      <c r="C13" t="s">
-        <v>27</v>
-      </c>
       <c r="D13" t="s">
         <v>23</v>
       </c>
       <c r="E13" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="F13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+      <c r="G13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="B14">
         <v>6.7204E-2</v>
       </c>
-      <c r="C14" t="s">
-        <v>30</v>
-      </c>
       <c r="D14" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E14" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="F14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>31</v>
+        <v>24</v>
+      </c>
+      <c r="G14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="B15">
         <v>9.7446000000000002E-4</v>
       </c>
-      <c r="C15" t="s">
-        <v>35</v>
-      </c>
       <c r="D15" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="E15" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+      <c r="G15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="B16">
         <v>0.17136999999999999</v>
       </c>
-      <c r="C16" t="s">
-        <v>34</v>
-      </c>
       <c r="D16" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E16" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+      <c r="G16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="2"/>
-    </row>
-    <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>3</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C19" s="2"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -1615,7 +1693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -1623,7 +1701,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -1631,12 +1709,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>11</v>
       </c>
@@ -1644,131 +1722,138 @@
         <v>12</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="G26" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B27" s="3">
         <v>1</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>35</v>
-      </c>
+      <c r="C27" s="3"/>
       <c r="D27" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E27" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E27" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F27" t="s">
+      <c r="F27" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G27" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B28">
         <v>1</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>9</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="E28" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E28" t="s">
-        <v>47</v>
-      </c>
       <c r="F28" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+      <c r="G28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B29">
         <v>0.01</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>9</v>
       </c>
-      <c r="D29" t="s">
-        <v>23</v>
-      </c>
       <c r="E29" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="F29" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="G29" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="B30">
         <v>0.05</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>9</v>
       </c>
-      <c r="D30" t="s">
-        <v>23</v>
-      </c>
       <c r="E30" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="F30" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+      <c r="G30" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
-    </row>
-    <row r="32" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="E31" s="5"/>
+    </row>
+    <row r="32" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C32" s="2"/>
-    </row>
-    <row r="33" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+      <c r="C32" s="3"/>
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>3</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C33" s="2"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+      <c r="C33" s="3"/>
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>4</v>
       </c>
       <c r="B34" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>5</v>
       </c>
@@ -1776,7 +1861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>6</v>
       </c>
@@ -1784,7 +1869,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>8</v>
       </c>
@@ -1792,12 +1877,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>11</v>
       </c>
@@ -1805,129 +1890,136 @@
         <v>12</v>
       </c>
       <c r="C40" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="E40" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="F40" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="G40" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B41" s="3">
         <v>1</v>
       </c>
-      <c r="C41" s="3" t="s">
-        <v>35</v>
-      </c>
+      <c r="C41" s="3"/>
       <c r="D41" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E41" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E41" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F41" t="s">
+      <c r="F41" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G41" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B42">
         <v>1</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
         <v>9</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="E42" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E42" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F42" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A43" s="3" t="s">
-        <v>52</v>
+      <c r="F42" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G42" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>49</v>
       </c>
       <c r="B43">
         <v>1.6</v>
       </c>
-      <c r="C43" t="s">
-        <v>30</v>
-      </c>
       <c r="D43" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E43" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="F43" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
-        <v>51</v>
+        <v>43</v>
+      </c>
+      <c r="G43" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A44" s="8" t="s">
+        <v>56</v>
       </c>
       <c r="B44">
         <v>8</v>
       </c>
-      <c r="C44" t="s">
-        <v>30</v>
-      </c>
       <c r="D44" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E44" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="F44" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="G44" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="5"/>
       <c r="B45" s="5"/>
-    </row>
-    <row r="46" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="C45" s="5"/>
+    </row>
+    <row r="46" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C46" s="2"/>
-    </row>
-    <row r="47" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+      <c r="C46" s="3"/>
+      <c r="D46" s="2"/>
+    </row>
+    <row r="47" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>3</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C47" s="2"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="C47" s="3"/>
+      <c r="D47" s="2"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>4</v>
       </c>
       <c r="B48" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>5</v>
       </c>
@@ -1935,7 +2027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>6</v>
       </c>
@@ -1943,7 +2035,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>8</v>
       </c>
@@ -1951,12 +2043,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>11</v>
       </c>
@@ -1964,127 +2056,136 @@
         <v>12</v>
       </c>
       <c r="C54" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="E54" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="1" t="s">
+      <c r="F54" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F54" s="1" t="s">
+      <c r="G54" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B55" s="3">
         <v>1</v>
       </c>
-      <c r="C55" s="3" t="s">
-        <v>35</v>
-      </c>
+      <c r="C55" s="3"/>
       <c r="D55" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E55" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E55" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F55" t="s">
+      <c r="F55" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G55" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B56">
         <v>0.7</v>
       </c>
-      <c r="C56" t="s">
+      <c r="D56" t="s">
         <v>9</v>
       </c>
-      <c r="D56" s="3" t="s">
+      <c r="E56" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E56" t="s">
-        <v>24</v>
-      </c>
       <c r="F56" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+      <c r="G56" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B57" s="5">
         <v>1.296</v>
       </c>
-      <c r="C57" t="s">
-        <v>27</v>
-      </c>
+      <c r="C57" s="5"/>
       <c r="D57" t="s">
         <v>23</v>
       </c>
       <c r="E57" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F57" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58" s="5" t="s">
-        <v>31</v>
+        <v>22</v>
+      </c>
+      <c r="G57" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A58" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="B58" s="5">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C58" t="s">
-        <v>35</v>
-      </c>
+      <c r="C58" s="5"/>
       <c r="D58" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="E58" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F58" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A59" s="4" t="s">
-        <v>55</v>
+        <v>22</v>
+      </c>
+      <c r="G58" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A59" s="7" t="s">
+        <v>58</v>
       </c>
       <c r="B59" s="4">
         <v>0.42</v>
       </c>
-      <c r="C59" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D59" t="s">
-        <v>23</v>
+      <c r="C59" s="4"/>
+      <c r="D59" s="5" t="s">
+        <v>59</v>
       </c>
       <c r="E59" t="s">
+        <v>42</v>
+      </c>
+      <c r="F59" t="s">
         <v>24</v>
       </c>
-      <c r="F59" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="G59" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
-      <c r="C60" s="5"/>
-    </row>
-    <row r="61" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="C60" s="4"/>
+      <c r="D60" s="5"/>
+    </row>
+    <row r="61" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="4"/>
       <c r="B61" s="5"/>
-      <c r="C61" s="4"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>